<commit_message>
add Date to excel
</commit_message>
<xml_diff>
--- a/src/test/resources/EurotechTest.xlsx
+++ b/src/test/resources/EurotechTest.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zeynepusta/IdeaProjects/EuroTech-SDET6/Batch6TestNGSelenium/src/test/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CEDF91-C602-5640-9DD0-7526AAC09704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="39320" yWindow="3000" windowWidth="28800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39320" yWindow="3000" windowWidth="28800" windowHeight="16280"/>
   </bookViews>
   <sheets>
     <sheet name="Test Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
   <si>
     <t>Username</t>
   </si>
@@ -192,12 +186,22 @@
   </si>
   <si>
     <t>Tester</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>2022/01/02 - Now</t>
+  </si>
+  <si>
+    <t>2022/03/03 - Now</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -278,7 +282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -301,10 +305,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -615,23 +620,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="23" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="23" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="29.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="6" width="32.6640625"/>
+    <col min="2" max="2" customWidth="true" style="6" width="23.6640625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="6" width="29.83203125"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="6" width="13.6640625"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="6" width="16.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -647,8 +652,11 @@
       <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="F1" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -664,8 +672,11 @@
       <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="F2" t="s" s="0">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -681,8 +692,11 @@
       <c r="E3" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="F3" t="s" s="0">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -699,7 +713,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -716,7 +730,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
@@ -733,7 +747,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
@@ -750,7 +764,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
@@ -767,7 +781,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>38</v>
       </c>
@@ -784,7 +798,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>40</v>
       </c>
@@ -801,7 +815,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>44</v>
       </c>
@@ -818,7 +832,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>48</v>
       </c>
@@ -836,8 +850,9 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>